<commit_message>
add feature ( save Item table ) only one row. need to develope adding row.
</commit_message>
<xml_diff>
--- a/bin/Database Structure.xlsx
+++ b/bin/Database Structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="195" yWindow="75" windowWidth="23250" windowHeight="13110" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2676" windowWidth="22620" windowHeight="6744" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="DATABASE" sheetId="7" r:id="rId1"/>
@@ -18,11 +18,12 @@
     <sheet name="정규화" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A13:H27"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="604">
   <si>
     <t>RMA number</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2007,6 +2008,22 @@
   </si>
   <si>
     <t>ItemName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">company와 site쪽에도 검색 항목 바로 완성이아니라 고를 수있도록 구현.. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한글 저장안됨..</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2423,10 +2440,10 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="4" max="4" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.8984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2499,14 +2516,14 @@
       <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2598,16 +2615,16 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="2" max="2" width="28.125" customWidth="1"/>
-    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.09765625" customWidth="1"/>
+    <col min="3" max="3" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -2708,11 +2725,11 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.875" customWidth="1"/>
-    <col min="5" max="5" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.8984375" customWidth="1"/>
+    <col min="5" max="5" width="11.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -7596,13 +7613,13 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
     <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.375" customWidth="1"/>
-    <col min="5" max="5" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.3984375" customWidth="1"/>
+    <col min="5" max="5" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16384">
@@ -24119,24 +24136,24 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.875" customWidth="1"/>
+    <col min="1" max="1" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.8984375" customWidth="1"/>
     <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.09765625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="38" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.8984375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.8984375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -24254,7 +24271,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="16.899999999999999" customHeight="1">
+    <row r="19" spans="2:7" ht="16.95" customHeight="1">
       <c r="B19" s="1" t="s">
         <v>45</v>
       </c>
@@ -24310,13 +24327,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -24347,23 +24364,23 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A3:H33"/>
+  <dimension ref="A3:H42"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="13.625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="4.125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="42.125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="8.75" style="9"/>
-    <col min="5" max="5" width="8.75" style="6"/>
-    <col min="6" max="6" width="47.25" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.25" style="6" customWidth="1"/>
-    <col min="8" max="8" width="24.125" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="8.75" style="6"/>
+    <col min="1" max="1" width="13.59765625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="4.09765625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="42.09765625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="8.69921875" style="9"/>
+    <col min="5" max="5" width="8.69921875" style="6"/>
+    <col min="6" max="6" width="47.19921875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.19921875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="24.09765625" style="6" customWidth="1"/>
+    <col min="9" max="16384" width="8.69921875" style="6"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:8">
@@ -24377,7 +24394,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="33">
+    <row r="5" spans="1:8" ht="34.799999999999997">
       <c r="A5" s="7">
         <v>42816</v>
       </c>
@@ -24394,7 +24411,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="49.5">
+    <row r="6" spans="1:8" ht="52.2">
       <c r="B6" s="8" t="s">
         <v>110</v>
       </c>
@@ -24411,7 +24428,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="99">
+    <row r="7" spans="1:8" ht="104.4">
       <c r="B7" s="8" t="s">
         <v>112</v>
       </c>
@@ -24431,7 +24448,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="33">
+    <row r="9" spans="1:8">
       <c r="A9" s="7">
         <v>42817</v>
       </c>
@@ -24456,7 +24473,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="49.5">
+    <row r="12" spans="1:8" ht="34.799999999999997">
       <c r="A12" s="7">
         <v>42818</v>
       </c>
@@ -24484,7 +24501,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="33">
+    <row r="16" spans="1:8" ht="34.799999999999997">
       <c r="B16" s="8" t="s">
         <v>173</v>
       </c>
@@ -24503,76 +24520,95 @@
         <v>176</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="C24" s="6" t="s">
+    <row r="20" spans="1:3" ht="34.799999999999997">
+      <c r="A20" s="7">
+        <v>42846</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>600</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="B21" s="8" t="s">
+        <v>602</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="C33" s="6" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="7">
+    <row r="34" spans="1:3">
+      <c r="A34" s="7">
         <v>42816</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B34" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C34" s="6" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="B26" s="8" t="s">
+    <row r="35" spans="1:3">
+      <c r="B35" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C35" s="6" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="B27" s="8" t="s">
+    <row r="36" spans="1:3">
+      <c r="B36" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C36" s="6" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="33">
-      <c r="B28" s="8" t="s">
+    <row r="37" spans="1:3" ht="34.799999999999997">
+      <c r="B37" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C37" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="33">
-      <c r="B29" s="8" t="s">
+    <row r="38" spans="1:3" ht="34.799999999999997">
+      <c r="B38" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C38" s="10" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="C30" s="10"/>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="C31" s="10"/>
-    </row>
-    <row r="32" spans="1:3" ht="49.5">
-      <c r="A32" s="7">
+    <row r="39" spans="1:3">
+      <c r="C39" s="10"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="C40" s="10"/>
+    </row>
+    <row r="41" spans="1:3" ht="52.2">
+      <c r="A41" s="7">
         <v>42817</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B41" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C41" s="6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="33" spans="2:3">
-      <c r="B33" s="8" t="s">
+    <row r="42" spans="1:3">
+      <c r="B42" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C42" s="6" t="s">
         <v>116</v>
       </c>
     </row>
@@ -24581,7 +24617,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B1:B12 B14 B19:B1048576 B17" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:B12 B14 B19 B17 B30:B1048576" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -24595,9 +24631,9 @@
       <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.25" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="18.19921875" defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="16384" width="18.25" style="11"/>
+    <col min="1" max="16384" width="18.19921875" style="11"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:19" ht="29.25" customHeight="1">

</xml_diff>

<commit_message>
History Panel BackGround Bug fix.
</commit_message>
<xml_diff>
--- a/bin/Database Structure.xlsx
+++ b/bin/Database Structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2676" windowWidth="22620" windowHeight="6744" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="2640" windowWidth="22200" windowHeight="6480" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="DATABASE" sheetId="7" r:id="rId1"/>
@@ -18,11 +18,12 @@
     <sheet name="정규화" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="607">
   <si>
     <t>RMA number</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2023,6 +2024,18 @@
   </si>
   <si>
     <t>한글 저장안됨..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">선택했을때 배경에 뭐가 남음.. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>걍 불투명 포기함 ㅋ 짜증나!!!</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2439,10 +2452,10 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="4" max="4" width="20.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2515,14 +2528,14 @@
       <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.09765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2618,12 +2631,12 @@
       <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="2" max="2" width="28.09765625" customWidth="1"/>
-    <col min="3" max="3" width="11.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.09765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" customWidth="1"/>
+    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -2724,11 +2737,11 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.8984375" customWidth="1"/>
-    <col min="5" max="5" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.875" customWidth="1"/>
+    <col min="5" max="5" width="11.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -7612,13 +7625,13 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.3984375" customWidth="1"/>
-    <col min="5" max="5" width="11.8984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.375" customWidth="1"/>
+    <col min="5" max="5" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16384">
@@ -24135,24 +24148,24 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.8984375" customWidth="1"/>
+    <col min="1" max="1" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.875" customWidth="1"/>
     <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.69921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="38" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.8984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.8984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.59765625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -24270,7 +24283,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="16.95" customHeight="1">
+    <row r="19" spans="2:7" ht="16.899999999999999" customHeight="1">
       <c r="B19" s="1" t="s">
         <v>45</v>
       </c>
@@ -24329,10 +24342,10 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="12.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -24365,21 +24378,21 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A3:H42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="13.59765625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="4.09765625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="42.09765625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="8.69921875" style="9"/>
-    <col min="5" max="5" width="8.69921875" style="6"/>
-    <col min="6" max="6" width="47.19921875" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.19921875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="24.09765625" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="8.69921875" style="6"/>
+    <col min="1" max="1" width="13.625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="4.125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="42.125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="8.75" style="9"/>
+    <col min="5" max="5" width="8.75" style="6"/>
+    <col min="6" max="6" width="47.25" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.25" style="6" customWidth="1"/>
+    <col min="8" max="8" width="24.125" style="6" customWidth="1"/>
+    <col min="9" max="16384" width="8.75" style="6"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:8">
@@ -24393,7 +24406,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="34.799999999999997">
+    <row r="5" spans="1:8" ht="33">
       <c r="A5" s="7">
         <v>42816</v>
       </c>
@@ -24410,7 +24423,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="52.2">
+    <row r="6" spans="1:8" ht="49.5">
       <c r="B6" s="8" t="s">
         <v>110</v>
       </c>
@@ -24427,7 +24440,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="104.4">
+    <row r="7" spans="1:8" ht="99">
       <c r="B7" s="8" t="s">
         <v>112</v>
       </c>
@@ -24447,7 +24460,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" ht="33">
       <c r="A9" s="7">
         <v>42817</v>
       </c>
@@ -24472,7 +24485,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="34.799999999999997">
+    <row r="12" spans="1:8" ht="49.5">
       <c r="A12" s="7">
         <v>42818</v>
       </c>
@@ -24500,7 +24513,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="34.799999999999997">
+    <row r="16" spans="1:8" ht="33">
       <c r="B16" s="8" t="s">
         <v>173</v>
       </c>
@@ -24508,7 +24521,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:4">
       <c r="A18" s="7">
         <v>42825</v>
       </c>
@@ -24519,7 +24532,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="34.799999999999997">
+    <row r="20" spans="1:4" ht="33">
       <c r="A20" s="7">
         <v>42846</v>
       </c>
@@ -24530,12 +24543,26 @@
         <v>601</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:4">
       <c r="B21" s="8" t="s">
         <v>602</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>603</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="49.5">
+      <c r="A23" s="7">
+        <v>42857</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>604</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>606</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -24570,7 +24597,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="34.799999999999997">
+    <row r="37" spans="1:3" ht="33">
       <c r="B37" s="8" t="s">
         <v>113</v>
       </c>
@@ -24578,7 +24605,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="34.799999999999997">
+    <row r="38" spans="1:3" ht="33">
       <c r="B38" s="8" t="s">
         <v>114</v>
       </c>
@@ -24592,7 +24619,7 @@
     <row r="40" spans="1:3">
       <c r="C40" s="10"/>
     </row>
-    <row r="41" spans="1:3" ht="52.2">
+    <row r="41" spans="1:3" ht="49.5">
       <c r="A41" s="7">
         <v>42817</v>
       </c>
@@ -24630,9 +24657,9 @@
       <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.19921875" defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultColWidth="18.25" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="16384" width="18.19921875" style="11"/>
+    <col min="1" max="16384" width="18.25" style="11"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:19" ht="29.25" customHeight="1">

</xml_diff>

<commit_message>
Item table 저장 완료
</commit_message>
<xml_diff>
--- a/bin/Database Structure.xlsx
+++ b/bin/Database Structure.xlsx
@@ -18,12 +18,11 @@
     <sheet name="정규화" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="616">
   <si>
     <t>RMA number</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2035,7 +2034,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>1.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>걍 불투명 포기함 ㅋ 짜증나!!!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>완료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clear 햇을때 order number 삭제 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">history 클릭했을때 site 불러오기. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Clear와 New의 기능 구분이 안됨. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저장했을때 히스토리 갱신</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -24376,17 +24411,18 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A3:H42"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="13.625" style="7" customWidth="1"/>
     <col min="2" max="2" width="4.125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="42.125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="66.625" style="6" customWidth="1"/>
     <col min="4" max="4" width="8.75" style="9"/>
     <col min="5" max="5" width="8.75" style="6"/>
     <col min="6" max="6" width="47.25" style="6" bestFit="1" customWidth="1"/>
@@ -24395,246 +24431,299 @@
     <col min="9" max="16384" width="8.75" style="6"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8">
-      <c r="C3" s="9" t="s">
+    <row r="1" spans="1:8" ht="30" customHeight="1">
+      <c r="C1" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="33">
-      <c r="A5" s="7">
+    <row r="3" spans="1:8" ht="30" customHeight="1">
+      <c r="A3" s="7">
         <v>42816</v>
       </c>
+      <c r="B3" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" customHeight="1">
+      <c r="B4" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" customHeight="1">
       <c r="B5" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>101</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="49.5">
-      <c r="B6" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" customHeight="1">
+      <c r="A7" s="7">
+        <v>42817</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" customHeight="1">
+      <c r="B8" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="99">
-      <c r="B7" s="8" t="s">
+      <c r="C8" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" customHeight="1">
+      <c r="A10" s="7">
+        <v>42818</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" customHeight="1">
+      <c r="A13" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30" customHeight="1">
+      <c r="B14" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30" customHeight="1">
+      <c r="A16" s="7">
+        <v>42825</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>608</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30" customHeight="1">
+      <c r="A18" s="7">
+        <v>42846</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>600</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" customHeight="1">
+      <c r="B19" s="8" t="s">
+        <v>602</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" customHeight="1">
+      <c r="A21" s="7">
+        <v>42857</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>604</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>608</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" customHeight="1">
+      <c r="A23" s="7">
+        <v>42858</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>606</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>609</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30" customHeight="1">
+      <c r="B24" s="8" t="s">
+        <v>610</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>611</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" customHeight="1">
+      <c r="B25" s="8" t="s">
+        <v>613</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="30" customHeight="1">
+      <c r="B26" s="8" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30" customHeight="1">
+      <c r="C32" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="30" customHeight="1">
+      <c r="A33" s="7">
+        <v>42816</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="30" customHeight="1">
+      <c r="B34" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="30" customHeight="1">
+      <c r="B35" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="33">
-      <c r="A9" s="7">
+      <c r="C35" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="30" customHeight="1">
+      <c r="B36" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="30" customHeight="1">
+      <c r="B37" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="30" customHeight="1">
+      <c r="C38" s="10"/>
+    </row>
+    <row r="39" spans="1:3" ht="30" customHeight="1">
+      <c r="C39" s="10"/>
+    </row>
+    <row r="40" spans="1:3" ht="30" customHeight="1">
+      <c r="A40" s="7">
         <v>42817</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B40" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="B10" s="8" t="s">
+      <c r="C40" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="30" customHeight="1">
+      <c r="B41" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="49.5">
-      <c r="A12" s="7">
-        <v>42818</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="33">
-      <c r="B16" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="7">
-        <v>42825</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="33">
-      <c r="A20" s="7">
-        <v>42846</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>600</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="B21" s="8" t="s">
-        <v>602</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="49.5">
-      <c r="A23" s="7">
-        <v>42857</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>604</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>605</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="C33" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="7">
-        <v>42816</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="B35" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="B36" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="33">
-      <c r="B37" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="33">
-      <c r="B38" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="C39" s="10"/>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="C40" s="10"/>
-    </row>
-    <row r="41" spans="1:3" ht="49.5">
-      <c r="A41" s="7">
-        <v>42817</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>111</v>
-      </c>
       <c r="C41" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="B42" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="C42" s="6" t="s">
         <v>116</v>
       </c>
     </row>
@@ -24643,7 +24732,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B1:B12 B14 B19 B17 B30:B1048576" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:B10 B12 B17 B15 B29:B1048576" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Select Box 업데이트 전
</commit_message>
<xml_diff>
--- a/bin/Database Structure.xlsx
+++ b/bin/Database Structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2640" windowWidth="22200" windowHeight="6480" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="2640" windowWidth="22200" windowHeight="6480" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="DATABASE" sheetId="7" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="627">
   <si>
     <t>RMA number</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2071,6 +2071,50 @@
   </si>
   <si>
     <t>4.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Item은 존재하는 ITEM 이름과 일치해야만 함. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>버그 존재. 아이템 항목에서 뭐가하나 빠졋을때.. 에러남</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일 첨부하는 기능.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>save 동작할때 item을 수정하도록 변경 제어 가능하도록..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RMA 정보 저장할때 날짜 저장될수 있도록.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>숫자형식</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DA 추가한 형식</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -24177,10 +24221,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -24254,110 +24298,118 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
-      <c r="B7" s="1" t="s">
-        <v>52</v>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>625</v>
+      </c>
+      <c r="B4" t="s">
+        <v>626</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="B8" s="1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="B9" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="B12" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="B13" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" s="2"/>
+        <v>49</v>
+      </c>
     </row>
     <row r="14" spans="1:11">
       <c r="B14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="B15" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
-      <c r="B15" s="3" t="s">
+    <row r="16" spans="1:11">
+      <c r="B16" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
-      <c r="B16" s="1" t="s">
+    <row r="17" spans="2:2">
+      <c r="B17" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="2:7">
-      <c r="B17" s="1" t="s">
+    <row r="18" spans="2:2">
+      <c r="B18" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
-      <c r="B18" s="1" t="s">
+    <row r="19" spans="2:2">
+      <c r="B19" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="16.899999999999999" customHeight="1">
-      <c r="B19" s="1" t="s">
+    <row r="20" spans="2:2" ht="16.899999999999999" customHeight="1">
+      <c r="B20" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="2:7">
-      <c r="B20" s="1" t="s">
+    <row r="21" spans="2:2">
+      <c r="B21" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="2:7">
-      <c r="B23" t="s">
+    <row r="24" spans="2:2">
+      <c r="B24" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="2:7">
-      <c r="B24" t="s">
+    <row r="25" spans="2:2">
+      <c r="B25" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="2:7">
-      <c r="B25" t="s">
+    <row r="26" spans="2:2">
+      <c r="B26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="2:7">
-      <c r="B28" t="s">
+    <row r="29" spans="2:2">
+      <c r="B29" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="2:7">
-      <c r="B31" t="s">
+    <row r="32" spans="2:2">
+      <c r="B32" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="2:7">
-      <c r="B32" t="s">
+    <row r="33" spans="2:7">
+      <c r="B33" t="s">
         <v>91</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G33" t="s">
         <v>92</v>
       </c>
     </row>
@@ -24411,11 +24463,11 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="30" customHeight="1"/>
@@ -24653,77 +24705,118 @@
       <c r="B26" s="8" t="s">
         <v>615</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" ht="30" customHeight="1">
-      <c r="C32" s="6" t="s">
+      <c r="C26" s="6" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="30" customHeight="1">
+      <c r="B27" s="8" t="s">
+        <v>617</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" customHeight="1">
+      <c r="B28" s="8" t="s">
+        <v>619</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" customHeight="1">
+      <c r="A30" s="7">
+        <v>42865</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>621</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30" customHeight="1">
+      <c r="A31" s="7">
+        <v>42867</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>623</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="30" customHeight="1">
+      <c r="C34" s="6" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="30" customHeight="1">
-      <c r="A33" s="7">
+    <row r="35" spans="1:3" ht="30" customHeight="1">
+      <c r="A35" s="7">
         <v>42816</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B35" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C35" s="6" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="30" customHeight="1">
-      <c r="B34" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="30" customHeight="1">
-      <c r="B35" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="30" customHeight="1">
       <c r="B36" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="30" customHeight="1">
       <c r="B37" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="30" customHeight="1">
+      <c r="B38" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="30" customHeight="1">
+      <c r="B39" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C39" s="10" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" customHeight="1">
-      <c r="C38" s="10"/>
-    </row>
-    <row r="39" spans="1:3" ht="30" customHeight="1">
-      <c r="C39" s="10"/>
-    </row>
     <row r="40" spans="1:3" ht="30" customHeight="1">
-      <c r="A40" s="7">
+      <c r="C40" s="10"/>
+    </row>
+    <row r="41" spans="1:3" ht="30" customHeight="1">
+      <c r="C41" s="10"/>
+    </row>
+    <row r="42" spans="1:3" ht="30" customHeight="1">
+      <c r="A42" s="7">
         <v>42817</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B42" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C42" s="6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" customHeight="1">
-      <c r="B41" s="8" t="s">
+    <row r="43" spans="1:3" ht="30" customHeight="1">
+      <c r="B43" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C43" s="6" t="s">
         <v>116</v>
       </c>
     </row>
@@ -24732,7 +24825,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B1:B10 B12 B17 B15 B29:B1048576" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:B10 B12 B17 B15 B33:B1048576" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
User Info 저장 가능
</commit_message>
<xml_diff>
--- a/bin/Database Structure.xlsx
+++ b/bin/Database Structure.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="663">
   <si>
     <t>RMA number</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2629,6 +2629,14 @@
   </si>
   <si>
     <t>RMA 테이블에 로그인 ID함께 저장.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>완료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">List만들어서 거기다가 파일 이름 추가함. </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3156,7 +3164,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="30" customHeight="1"/>
@@ -3465,7 +3473,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="30" customHeight="1">
+    <row r="33" spans="1:6" ht="30" customHeight="1">
       <c r="B33" s="8" t="s">
         <v>638</v>
       </c>
@@ -3476,7 +3484,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" customHeight="1">
+    <row r="35" spans="1:6" ht="30" customHeight="1">
       <c r="A35" s="7">
         <v>42902</v>
       </c>
@@ -3487,15 +3495,21 @@
         <v>654</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="30" customHeight="1">
+    <row r="36" spans="1:6" ht="30" customHeight="1">
       <c r="B36" s="8" t="s">
         <v>655</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>656</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="30" customHeight="1">
+      <c r="D36" s="9" t="s">
+        <v>661</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="30" customHeight="1">
       <c r="B37" s="8" t="s">
         <v>657</v>
       </c>
@@ -3503,7 +3517,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30" customHeight="1">
+    <row r="38" spans="1:6" ht="30" customHeight="1">
       <c r="B38" s="8" t="s">
         <v>659</v>
       </c>
@@ -3511,12 +3525,12 @@
         <v>660</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" customHeight="1">
+    <row r="43" spans="1:6" ht="30" customHeight="1">
       <c r="C43" s="6" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="30" customHeight="1">
+    <row r="44" spans="1:6" ht="30" customHeight="1">
       <c r="A44" s="7">
         <v>42816</v>
       </c>
@@ -3527,7 +3541,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="30" customHeight="1">
+    <row r="45" spans="1:6" ht="30" customHeight="1">
       <c r="B45" s="8" t="s">
         <v>109</v>
       </c>
@@ -3535,7 +3549,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="30" customHeight="1">
+    <row r="46" spans="1:6" ht="30" customHeight="1">
       <c r="B46" s="8" t="s">
         <v>111</v>
       </c>
@@ -3543,7 +3557,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="30" customHeight="1">
+    <row r="47" spans="1:6" ht="30" customHeight="1">
       <c r="B47" s="8" t="s">
         <v>112</v>
       </c>
@@ -3551,7 +3565,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="30" customHeight="1">
+    <row r="48" spans="1:6" ht="30" customHeight="1">
       <c r="B48" s="8" t="s">
         <v>113</v>
       </c>

</xml_diff>